<commit_message>
Initial Glider Design v5.1
- Python
- Integrate roll damping in roll-in kinematic model
- Consistent PEP 8 Style Python formatting
</commit_message>
<xml_diff>
--- a/01_Initial_Glider_Design/results/Nausicaa_v_5_0/nausicaa_results.xlsx
+++ b/01_Initial_Glider_Design/results/Nausicaa_v_5_0/nausicaa_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.327784112127733</v>
+        <v>5.141061488811325</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.00000003855841</v>
+        <v>10.00000009984927</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>64.99999949623385</v>
+        <v>65.00000064741765</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.349263547398809</v>
+        <v>1.256345602990154</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.366201538537022</v>
+        <v>2.366201640490309</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07770138350981098</v>
+        <v>0.08277678496321403</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.435919453737733</v>
+        <v>8.087660995770321</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.695366797949263</v>
+        <v>1.504116959381735</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.694745676970213</v>
+        <v>1.41925860399273</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.0006211209790496497</v>
+        <v>-0.08485835538900477</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04000001085452119</v>
+        <v>0.03999999052013917</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4970824407356021</v>
+        <v>0.3999999900529829</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.019999992869279</v>
+        <v>0.01999999000524018</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>51829.43367381862</v>
+        <v>49463.23004659176</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.07029593134557896</v>
+        <v>-0.1015359301217917</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.67682964941654</v>
+        <v>0.8056713410028052</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.7075564656005838</v>
+        <v>0.8114614932330131</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.189942846098154</v>
+        <v>2.053750223110356</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1421008585876863</v>
+        <v>0.1405388941750224</v>
       </c>
     </row>
     <row r="21">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1005443812611117</v>
+        <v>0.1140419009245801</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.67682964941654</v>
+        <v>0.8056713410028052</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.2048716065116614</v>
+        <v>0.1784068470692191</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.05121790162791536</v>
+        <v>0.04460171176730478</v>
       </c>
     </row>
     <row r="26">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.01049309378866726</v>
+        <v>0.007957250770294935</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.67682964941654</v>
+        <v>0.8056713410028052</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.06484099722250292</v>
+        <v>0.0677824264146713</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.03242049861125146</v>
+        <v>0.03389121320733565</v>
       </c>
     </row>
     <row r="31">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.002102177460404316</v>
+        <v>0.002297228665330165</v>
       </c>
     </row>
     <row r="33">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-3.55503935295126e-16</v>
+        <v>-1.32197450498956e-15</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>8.3058287654408e-15</v>
+        <v>1.608227095629997e-14</v>
       </c>
     </row>
     <row r="38">
@@ -812,393 +812,393 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>7.753597763039664</v>
+        <v>10.00580694562281</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>objective_total</t>
+          <t>p_roll (rad/s)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.01037425926732823</v>
+        <v>1.055098752613763</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>objective_sink</t>
+          <t>p_roll (deg/s)</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>60.45270549428633</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>objective_climb</t>
+          <t>p_roll_max (rad/s)</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3.857912706155953e-07</v>
+        <v>13.61794718233036</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>objective_mass</t>
+          <t>t_roll (s)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>1.075220705441564</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>objective_span</t>
+          <t>psi_0 (deg)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.009772690693347482</v>
+        <v>-31.60949773307858</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>objective_control</t>
+          <t>Cl_da (rad^-1)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.000601182782710137</v>
+        <v>-0.4866281482559692</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>penalty</t>
+          <t>objective_total</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>6.754696767705246e-11</v>
+        <v>1.065901365071977</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>x_cg (m)</t>
+          <t>objective_climb</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.03697010460049686</v>
+        <v>0.007249436628742574</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>y_cg (m)</t>
+          <t>objective_span</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-5.886610647795852e-21</v>
+        <v>1.057650766716904</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>z_cg (m)</t>
+          <t>objective_control</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.002810779761746139</v>
+        <v>0.001001161726330736</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>I_xx (kg m^2)</t>
+          <t>penalty</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.001321262969359352</v>
+        <v>3.333585406817299e-10</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>I_yy (kg m^2)</t>
+          <t>x_cg (m)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.001312085616816881</v>
+        <v>0.03284266895196183</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>I_zz (kg m^2)</t>
+          <t>y_cg (m)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.002630358209185406</v>
+        <v>-1.27227663362964e-17</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>I_xy (kg m^2)</t>
+          <t>z_cg (m)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2.809568651347573e-22</v>
+        <v>0.003182731310932615</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>I_xz (kg m^2)</t>
+          <t>I_xx (kg m^2)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-2.382220141880354e-06</v>
+        <v>0.001945924981276573</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>I_yz (kg m^2)</t>
+          <t>I_yy (kg m^2)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-1.374481947695079e-21</v>
+        <v>0.001961788971508408</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>mass_wing_kg</t>
+          <t>I_zz (kg m^2)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.0293263712386249</v>
+        <v>0.003903935294542807</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>mass_htail_surfaces_kg</t>
+          <t>I_xy (kg m^2)</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.0009719745691682078</v>
+        <v>1.387152435409648e-21</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>mass_vtail_surfaces_kg</t>
+          <t>I_xz (kg m^2)</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.0001232589974190489</v>
+        <v>-4.48775121766283e-06</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>mass_linkages_kg</t>
+          <t>I_yz (kg m^2)</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.001</v>
+        <v>3.399195133571679e-21</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>mass_Receiver_kg</t>
+          <t>mass_wing_kg</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.005</v>
+        <v>0.03289764424912821</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>mass_battery_kg</t>
+          <t>mass_htail_surfaces_kg</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.013</v>
+        <v>0.0006418656542902716</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>mass_servo_kg</t>
+          <t>mass_vtail_surfaces_kg</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.0001408059179774253</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>mass_boom_kg</t>
+          <t>mass_linkages_kg</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.006724130226859071</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>mass_pod_kg</t>
+          <t>mass_Receiver_kg</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>mass_ballast_kg</t>
+          <t>mass_battery_kg</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-9.560024022146209e-09</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>mass_glue_weight_kg</t>
+          <t>mass_servo_kg</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.005755658037763777</v>
+        <v>0.008800000000000001</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>wing root LE x (m)</t>
+          <t>mass_boom_kg</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.03552521464692157</v>
+        <v>0.008164865440121372</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>wing root LE y (m)</t>
+          <t>mass_pod_kg</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>wing root LE z (m)</t>
+          <t>mass_ballast_kg</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>-9.99928206569716e-09</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>wing tip LE x (m)</t>
+          <t>mass_glue_weight_kg</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.03552521464692157</v>
+        <v>0.006131613700978818</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>wing tip LE y (m)</t>
+          <t>wing root LE x (m)</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.3535198470633772</v>
+        <v>-0.0351347235437556</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>wing tip LE z (m)</t>
+          <t>wing root LE y (m)</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.01351871797116486</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>htail root LE x (m)</t>
+          <t>wing root LE z (m)</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.6256117477886246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>htail root LE y (m)</t>
+          <t>wing tip LE x (m)</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>-0.0351347235437556</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>htail root LE z (m)</t>
+          <t>wing tip LE y (m)</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>0.4054701244165568</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>htail tip LE x (m)</t>
+          <t>wing tip LE z (m)</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.6256117477886246</v>
+        <v>0.01454018416698145</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>htail tip LE y (m)</t>
+          <t>htail root LE x (m)</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.1024358032558307</v>
+        <v>0.7610696292355005</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>htail tip LE z (m)</t>
+          <t>htail root LE y (m)</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1208,941 +1208,981 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>vtail root LE x (m)</t>
+          <t>htail root LE z (m)</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.6444091508052885</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>vtail root LE y (m)</t>
+          <t>htail tip LE x (m)</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>0.7610696292355005</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>vtail root LE z (m)</t>
+          <t>htail tip LE y (m)</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>0.08920342353460955</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>vtail tip LE x (m)</t>
+          <t>htail tip LE z (m)</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.6444091508052885</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>vtail tip LE y (m)</t>
+          <t>vtail root LE x (m)</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>0.7717801277954696</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>vtail tip LE z (m)</t>
+          <t>vtail root LE y (m)</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.06484099722250292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>aero_F_g[0]</t>
+          <t>vtail root LE z (m)</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.07432597049309683</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>aero_F_g[1]</t>
+          <t>vtail tip LE x (m)</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-8.467746404312084e-18</v>
+        <v>0.7717801277954696</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>aero_F_g[2]</t>
+          <t>vtail tip LE y (m)</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>1.81835683241096</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>aero_M_g[0]</t>
+          <t>vtail tip LE z (m)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>2.507399778193503e-19</v>
+        <v>0.0677824264146713</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>aero_M_g[1]</t>
+          <t>aero_F_g[0]</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>1.527543625444439e-10</v>
+        <v>-0.09968772864393802</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>aero_M_g[2]</t>
+          <t>aero_F_g[1]</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-5.194974581409206e-18</v>
+        <v>-1.642741440261673e-18</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>aero_F_b</t>
+          <t>aero_F_g[2]</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.07432597049309683</v>
+        <v>1.933514829369654</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>aero_F_w</t>
+          <t>aero_M_g[0]</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-0.2425575595184135</v>
+        <v>-8.192865265399014e-17</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>aero_M_b</t>
+          <t>aero_M_g[1]</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-2.507399778193503e-19</v>
+        <v>2.283188828972049e-14</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>aero_M_w</t>
+          <t>aero_M_g[2]</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>6.551671984133847e-19</v>
+        <v>-2.781845244806068e-17</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>aero_L</t>
+          <t>aero_F_b</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>1.803638475467251</v>
+        <v>0.09968772864393802</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>aero_Y</t>
+          <t>aero_F_w</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-8.467746404312084e-18</v>
+        <v>-0.2375780819118086</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>aero_D</t>
+          <t>aero_M_b</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.2425575595184135</v>
+        <v>8.192865265399014e-17</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>aero_l_b</t>
+          <t>aero_M_w</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-2.507399778193503e-19</v>
+        <v>8.551459592356331e-17</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>aero_m_b</t>
+          <t>aero_L</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>1.527543625444439e-10</v>
+        <v>1.92145098652806</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>aero_n_b</t>
+          <t>aero_Y</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>5.194974581409206e-18</v>
+        <v>-1.642741440261673e-18</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>aero_CL</t>
+          <t>aero_D</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>1.031793184228452</v>
+        <v>0.2375780819118086</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>aero_CY</t>
+          <t>aero_l_b</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-4.844076650937924e-18</v>
+        <v>8.192865265399014e-17</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>aero_CD</t>
+          <t>aero_m_b</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.1387579828764471</v>
+        <v>2.283188828972049e-14</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>aero_Cl</t>
+          <t>aero_n_b</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-2.027242221810846e-19</v>
+        <v>2.781845244806068e-17</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>aero_Cm</t>
+          <t>aero_CL</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>6.149503935126112e-10</v>
+        <v>1.040766902446284</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>aero_Cn</t>
+          <t>aero_CY</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>4.200156634078686e-18</v>
+        <v>-8.898019945804752e-19</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>wing_components_comp1_L (N)</t>
+          <t>aero_CD</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>1.715114867824261</v>
+        <v>0.1286857724366271</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>wing_components_comp1_D (N)</t>
+          <t>aero_Cl</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.0608079402996009</v>
+        <v>5.468800225985341e-17</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>wing_components_comp1_Y (N)</t>
+          <t>aero_Cm</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>8.799732308183184e-14</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>wing_components_comp1_l_b</t>
+          <t>aero_Cn</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-0</v>
+        <v>1.85690297724074e-17</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>wing_components_comp1_m_b</t>
+          <t>wing_components_comp1_L (N)</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.05557335582759033</v>
+        <v>1.854331488203392</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>wing_components_comp1_n_b</t>
+          <t>wing_components_comp1_D (N)</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-0</v>
+        <v>0.06870129053957613</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>wing_components_comp1_span_eff (m)</t>
+          <t>wing_components_comp1_Y (N)</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.7070398828415562</v>
+        <v>1.214306433183765e-17</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>wing_components_comp1_oswald</t>
+          <t>wing_components_comp1_l_b</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.8046853936055985</v>
+        <v>8.326672684688674e-17</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>wing_components_comp2_L (N)</t>
+          <t>wing_components_comp1_m_b</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.08682523749279589</v>
+        <v>0.05210876439358686</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>wing_components_comp2_D (N)</t>
+          <t>wing_components_comp1_n_b</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.03123937664807716</v>
+        <v>1.734723475976807e-17</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>wing_components_comp2_Y (N)</t>
+          <t>wing_components_comp1_span_eff (m)</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>0.8109404162444613</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>wing_components_comp2_l_b</t>
+          <t>wing_components_comp1_oswald</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-0</v>
+        <v>0.7998638959219753</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>wing_components_comp2_m_b</t>
+          <t>wing_components_comp2_L (N)</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-0.05500527234211582</v>
+        <v>0.06518784432553081</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>wing_components_comp2_n_b</t>
+          <t>wing_components_comp2_D (N)</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0</v>
+        <v>0.02827084386385509</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>wing_components_comp2_span_eff (m)</t>
+          <t>wing_components_comp2_Y (N)</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.2048716065116614</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>wing_components_comp2_oswald</t>
+          <t>wing_components_comp2_l_b</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.8106853777008906</v>
+        <v>-8.944667923005412e-19</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>wing_components_comp3_L (N)</t>
+          <t>wing_components_comp2_m_b</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0</v>
+        <v>-0.0513365394690181</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>wing_components_comp3_D (N)</t>
+          <t>wing_components_comp2_n_b</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.001104021871376682</v>
+        <v>2.236166980751353e-19</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>wing_components_comp3_Y (N)</t>
+          <t>wing_components_comp2_span_eff (m)</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-8.467746404312084e-18</v>
+        <v>0.1784068470692191</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>wing_components_comp3_l_b</t>
+          <t>wing_components_comp2_oswald</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-2.507287553958437e-19</v>
+        <v>0.8106853777008906</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>wing_components_comp3_m_b</t>
+          <t>wing_components_comp3_L (N)</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-8.542177806671748e-05</v>
+        <v>2.710505431213761e-20</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>wing_components_comp3_n_b</t>
+          <t>wing_components_comp3_D (N)</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>5.194968510018906e-18</v>
+        <v>0.001118499803066326</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>wing_components_comp3_span_eff (m)</t>
+          <t>wing_components_comp3_Y (N)</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.06484099722250292</v>
+        <v>-1.378580577209932e-17</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>wing_components_comp3_oswald</t>
+          <t>wing_components_comp3_l_b</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.8232692748986458</v>
+        <v>-4.161356364208345e-19</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_L (N)</t>
+          <t>wing_components_comp3_m_b</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.001698370150194115</v>
+        <v>-0.0001109254283730531</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_D (N)</t>
+          <t>wing_components_comp3_n_b</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.001346769153141628</v>
+        <v>1.023332831614988e-17</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_Y (N)</t>
+          <t>wing_components_comp3_span_eff (m)</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>0.0677824264146713</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_l_b</t>
+          <t>wing_components_comp3_oswald</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-1.122242350664079e-23</v>
+        <v>0.8232692748986458</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_m_b</t>
+          <t>fuselage_components_comp1_L (N)</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-0.0004826615546534318</v>
+        <v>0.001931653999137287</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_n_b</t>
+          <t>fuselage_components_comp1_D (N)</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>6.071390300345826e-24</v>
+        <v>0.001479730226077065</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_span_eff (m)</t>
+          <t>fuselage_components_comp1_Y (N)</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.004055451774444796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_oswald</t>
+          <t>fuselage_components_comp1_l_b</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.95</v>
+        <v>-2.747176417521673e-20</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>aero_D_profile</t>
+          <t>fuselage_components_comp1_m_b</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.09449810797219636</v>
+        <v>-0.0006612994961728788</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>aero_D_induced</t>
+          <t>fuselage_components_comp1_n_b</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.1480594515462171</v>
+        <v>1.427267406759412e-20</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>aero_CLa</t>
+          <t>fuselage_components_comp1_span_eff (m)</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>4.062710128886895</v>
+        <v>0.004055451774444796</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>aero_CDa</t>
+          <t>fuselage_components_comp1_oswald</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.802990130754007</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>aero_CYa</t>
+          <t>aero_D_profile</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>1.940380133451268e-22</v>
+        <v>0.09957036443257461</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>aero_Cla</t>
+          <t>aero_D_induced</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>-8.819727974977151e-23</v>
+        <v>0.138007717479234</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>aero_Cma</t>
+          <t>aero_CLa</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.162508449254249</v>
+        <v>4.021942757649293</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>aero_Cna</t>
+          <t>aero_CDa</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>-1.707741670887496e-22</v>
+        <v>0.7196226212826305</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>aero_x_np</t>
+          <t>aero_CYa</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.0426541404864411</v>
+        <v>2.785088802896838e-22</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>aero_CLb</t>
+          <t>aero_Cla</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>-5.233081117380457e-06</v>
+        <v>5.286877008665689e-13</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>aero_CDb</t>
+          <t>aero_Cma</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>-7.621754016471913e-07</v>
+        <v>-0.1608776721785141</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>aero_CYb</t>
+          <t>aero_Cna</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.1365729402246663</v>
+        <v>-2.325967398586828e-13</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>aero_Clb</t>
+          <t>aero_x_np</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-0.02500026678671</v>
+        <v>0.03846422338667357</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>aero_Cmb</t>
+          <t>aero_CLb</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>8.738172871279599e-07</v>
+        <v>-5.438646727552807e-06</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>aero_Cnb</t>
+          <t>aero_CDb</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.03152176543666309</v>
+        <v>-6.658968308846092e-07</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>aero_x_np_lateral</t>
+          <t>aero_CYb</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-0.1263377139554062</v>
+        <v>0.1396629135701793</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>aero_CLp</t>
+          <t>aero_Clb</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>-0.005691076799374528</v>
+        <v>-0.02499999015796307</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>aero_CDp</t>
+          <t>aero_Cmb</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>-0.00177941318968422</v>
+        <v>6.799741356075048e-07</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>aero_CYp</t>
+          <t>aero_Cnb</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>-0.08248418065954369</v>
+        <v>0.03217912956944434</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>aero_Clp</t>
+          <t>aero_x_np_lateral</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-0.6410368740334315</v>
+        <v>-0.1541226739859743</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>aero_Cmp</t>
+          <t>aero_CLp</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-0.001073786371678226</v>
+        <v>-0.00824421885603499</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>aero_Cnp</t>
+          <t>aero_CDp</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-0.2727539455789413</v>
+        <v>-0.001687347274764717</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>aero_CLq</t>
+          <t>aero_CYp</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.7694404472189387</v>
+        <v>-0.07811761689330377</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>aero_CDq</t>
+          <t>aero_Clp</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>1.239274279341673</v>
+        <v>-0.6462573293282363</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>aero_CYq</t>
+          <t>aero_Cmp</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-1.09109332188465e-17</v>
+        <v>-0.001214576490396257</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>aero_Clq</t>
+          <t>aero_Cnp</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>-3.931923858972538e-19</v>
+        <v>-0.2729271052282198</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>aero_Cmq</t>
+          <t>aero_CLq</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>-14.65270235727372</v>
+        <v>0.7477096696717478</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>aero_Cnq</t>
+          <t>aero_CDq</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>9.460530492838058e-18</v>
+        <v>1.261830316577978</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>aero_CLr</t>
+          <t>aero_CYq</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>-3.79546298834299e-05</v>
+        <v>-5.659664324254516e-15</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>aero_CDr</t>
+          <t>aero_Clq</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>-2.015505978780751e-05</v>
+        <v>-5.102221748878642e-14</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>aero_CYr</t>
+          <t>aero_Cmq</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.1148518852086742</v>
+        <v>-16.67366635714174</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>aero_Clr</t>
+          <t>aero_Cnq</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.2157427601370293</v>
+        <v>-1.155931116872107e-14</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>aero_Cmr</t>
+          <t>aero_CLr</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>-0.0002532456331992451</v>
+        <v>-0.0001276918786263792</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
+          <t>aero_CDr</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>-3.21477403031345e-05</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>aero_CYr</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0.1128903331499223</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>aero_Clr</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0.2225041885750886</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>aero_Cmr</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>-0.0002291904827817157</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
           <t>aero_Cnr</t>
         </is>
       </c>
-      <c r="B171" t="n">
-        <v>-0.06660213667519668</v>
+      <c r="B175" t="n">
+        <v>-0.07231340751734523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>